<commit_message>
Finalização da Landing Page e Footer
</commit_message>
<xml_diff>
--- a/Documentação/animes-psicologia.xlsx
+++ b/Documentação/animes-psicologia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xanda\OneDrive\Área de Trabalho\SPTECH\Projeto Individual\projeto_individual_primeiro_semestre\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC939DFA-188E-4137-8C4A-2369DAECF223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D2A18-13CA-437A-BA16-9655FBB75898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -944,7 +944,7 @@
                   <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>148</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1281,13 +1281,13 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>134</c:v>
+                        <c:v>155</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>92</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>42</c:v>
+                        <c:v>63</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2410,7 +2410,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="N2" s="1">
         <f>SUM(N3,N4,N5,N6)</f>
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="O2" s="7">
         <v>298</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="Q2" s="6">
         <f>SUM(Q3,Q4,Q5,Q6)</f>
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>118</v>
       </c>
       <c r="N4" s="1">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="O4" s="7">
         <f>O3-M4</f>
@@ -2622,11 +2622,11 @@
       </c>
       <c r="P4" s="6">
         <f>P3-N4</f>
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="Q4" s="6">
         <f>P4-O4</f>
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2900,28 +2900,28 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="17">
         <v>21</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="17">
         <v>2</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="18" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrando API e passando para WEB-DATA-VIZ
</commit_message>
<xml_diff>
--- a/Documentação/animes-psicologia.xlsx
+++ b/Documentação/animes-psicologia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xanda\OneDrive\Área de Trabalho\SPTECH\Projeto Individual\projeto_individual_primeiro_semestre\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D2A18-13CA-437A-BA16-9655FBB75898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A6C9FB-2068-4E16-A238-1DDC8F4D57BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,7 +1057,7 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>385</c:v>
+                        <c:v>393</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>92</c:v>
@@ -1069,7 +1069,7 @@
                         <c:v>60</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>115</c:v>
+                        <c:v>123</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1281,13 +1281,19 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>155</c:v>
+                        <c:v>189</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>92</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>21</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2410,7 +2416,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,14 +2513,14 @@
       </c>
       <c r="L2" s="1">
         <f>SUM(L3,L4,L5,L6)</f>
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="M2" s="1">
         <v>393</v>
       </c>
       <c r="N2" s="1">
         <f>SUM(N3,N4,N5,N6)</f>
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="O2" s="7">
         <v>298</v>
@@ -2664,7 +2670,9 @@
       <c r="M5" s="3">
         <v>60</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="3">
+        <v>13</v>
+      </c>
       <c r="O5" s="2">
         <f>O4-M5</f>
         <v>28</v>
@@ -2702,12 +2710,14 @@
       </c>
       <c r="L6" s="6">
         <f>SUM(E24:E31)</f>
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="M6" s="6">
         <v>115</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="6">
+        <v>21</v>
+      </c>
       <c r="O6" s="8">
         <f>O5-M6</f>
         <v>-87</v>
@@ -3108,54 +3118,54 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="17">
         <v>5</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="17">
         <v>3</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="17">
         <v>8</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="17">
         <v>3</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="18" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3290,28 +3300,28 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="16">
         <v>29</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="10">
-        <v>13</v>
-      </c>
-      <c r="F29" s="10">
+      <c r="E29" s="17">
+        <v>21</v>
+      </c>
+      <c r="F29" s="17">
         <v>2</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="18" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>